<commit_message>
Added all distribution types to the sample excel file being read in by the unit test
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
+++ b/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C482716-C21E-4315-9184-E2006E26BA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4544A01E-6DD7-4123-8D6E-5A721F199520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Internal</t>
   </si>
@@ -85,16 +85,49 @@
   </si>
   <si>
     <t>Beta PERT</t>
+  </si>
+  <si>
+    <t>The fourth test parameter</t>
+  </si>
+  <si>
+    <t>The fifth test parameter</t>
+  </si>
+  <si>
+    <t>The sixth test parameter</t>
+  </si>
+  <si>
+    <t>Test Parameter 4</t>
+  </si>
+  <si>
+    <t>Test Parameter 5</t>
+  </si>
+  <si>
+    <t>Test Parameter 6</t>
+  </si>
+  <si>
+    <t>Log Uniform</t>
+  </si>
+  <si>
+    <t>Truncated Normal</t>
+  </si>
+  <si>
+    <t>Truncated Log Normal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,27 +435,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>11</v>
       </c>
@@ -468,7 +501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>14</v>
       </c>
@@ -482,7 +515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -496,7 +529,50 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the distribution names to match what can be found in the enum
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
+++ b/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4544A01E-6DD7-4123-8D6E-5A721F199520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37732EA-DA0D-4ECB-A1C6-467A50FBC726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>Uniform</t>
   </si>
   <si>
-    <t>Beta PERT</t>
-  </si>
-  <si>
     <t>The fourth test parameter</t>
   </si>
   <si>
@@ -105,13 +102,16 @@
     <t>Test Parameter 6</t>
   </si>
   <si>
-    <t>Log Uniform</t>
-  </si>
-  <si>
-    <t>Truncated Normal</t>
-  </si>
-  <si>
-    <t>Truncated Log Normal</t>
+    <t>PERT</t>
+  </si>
+  <si>
+    <t>LogUniform</t>
+  </si>
+  <si>
+    <t>TruncatedNormal</t>
+  </si>
+  <si>
+    <t>TruncatedLogNormal</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,15 +526,15 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -545,10 +545,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -559,10 +559,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Added some values just to make sure they were being read correctly
</commit_message>
<xml_diff>
--- a/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
+++ b/Battelle.EPA.WideAreaDecon.API.Tests/InputFiles/ParameterTests/GenericParameter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\Battelle.EPA.WideAreaDecon.API.Tests\InputFiles\ParameterTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37732EA-DA0D-4ECB-A1C6-467A50FBC726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BB55D2-4258-4922-A1B5-6D341D635CED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,7 +438,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -500,6 +500,9 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -514,6 +517,12 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -528,6 +537,15 @@
       <c r="F4" t="s">
         <v>25</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -542,6 +560,12 @@
       <c r="F5" t="s">
         <v>26</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -556,6 +580,18 @@
       <c r="F6" t="s">
         <v>27</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -569,6 +605,18 @@
       </c>
       <c r="F7" t="s">
         <v>28</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>